<commit_message>
Fixed error in file generation for both student data and club data. See tests T3.7 and T3.7R.
</commit_message>
<xml_diff>
--- a/app/Export/StudentAnalysisCurrent.xlsx
+++ b/app/Export/StudentAnalysisCurrent.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE21"/>
+  <dimension ref="A1:AK21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,37 +421,37 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>00-2020</t>
+          <t>01-2020</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>01-2020</t>
+          <t>03-2020</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>02-2020</t>
+          <t>04-2020</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>03-2020</t>
+          <t>05-2020</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>04-2020</t>
+          <t>06-2020</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>06-2020</t>
+          <t>07-2020</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>07-2020</t>
+          <t>08-2020</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
@@ -476,82 +476,112 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
+          <t>13-2020</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>14-2020</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>15-2020</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>16-2020</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>17-2020</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>19-2020</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>20-2020</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>21-2020</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>22-2020</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>23-2020</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
         <is>
           <t>24-2020</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>25-2020</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
         <is>
           <t>26-2020</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>27-2020</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
         <is>
           <t>28-2020</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>29-2020</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>30-2020</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>31-2020</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>32-2020</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>33-2020</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>34-2020</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>35-2020</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>52-2021</t>
         </is>
       </c>
     </row>
@@ -574,47 +604,8 @@
           <t>N</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>1</v>
+      <c r="AJ2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -636,6 +627,12 @@
           <t>Y</t>
         </is>
       </c>
+      <c r="AJ3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -696,8 +693,8 @@
           <t>N</t>
         </is>
       </c>
-      <c r="AD6" t="n">
-        <v>1</v>
+      <c r="AJ6" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -879,66 +876,6 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" t="n">
-        <v>1</v>
-      </c>
-      <c r="K15" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" t="n">
-        <v>1</v>
-      </c>
-      <c r="N15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O15" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>1</v>
-      </c>
-      <c r="S15" t="n">
-        <v>1</v>
-      </c>
-      <c r="T15" t="n">
-        <v>1</v>
-      </c>
-      <c r="W15" t="n">
-        <v>1</v>
-      </c>
-      <c r="X15" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -959,6 +896,60 @@
           <t>N</t>
         </is>
       </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1</v>
+      </c>
+      <c r="U16" t="n">
+        <v>1</v>
+      </c>
+      <c r="V16" t="n">
+        <v>1</v>
+      </c>
+      <c r="X16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -979,9 +970,6 @@
           <t>N</t>
         </is>
       </c>
-      <c r="AE17" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1062,40 +1050,79 @@
           <t>N</t>
         </is>
       </c>
-      <c r="G21" t="n">
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
         <v>1</v>
       </c>
       <c r="J21" t="n">
         <v>1</v>
       </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
       <c r="L21" t="n">
         <v>1</v>
       </c>
+      <c r="M21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
       <c r="O21" t="n">
         <v>1</v>
       </c>
       <c r="P21" t="n">
         <v>1</v>
       </c>
+      <c r="Q21" t="n">
+        <v>1</v>
+      </c>
       <c r="R21" t="n">
         <v>1</v>
       </c>
       <c r="S21" t="n">
         <v>1</v>
       </c>
+      <c r="T21" t="n">
+        <v>1</v>
+      </c>
       <c r="U21" t="n">
         <v>1</v>
       </c>
       <c r="V21" t="n">
         <v>1</v>
       </c>
+      <c r="W21" t="n">
+        <v>1</v>
+      </c>
+      <c r="X21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>1</v>
+      </c>
       <c r="AA21" t="n">
         <v>1</v>
       </c>
-      <c r="AB21" t="n">
+      <c r="AD21" t="n">
         <v>1</v>
       </c>
       <c r="AE21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI21" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>